<commit_message>
"Added dataset and trained"
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -50,22 +50,89 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -358,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,30 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Enrollment</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>12 aug</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
-        <is>
-          <t>saksham</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>71</v>
-      </c>
-      <c r="C2" t="inlineStr">
         <is>
           <t>P</t>
         </is>
@@ -401,24 +450,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>rishi</t>
+          <t>P</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>67</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
-        <is>
-          <t>rohit</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>69</v>
-      </c>
-      <c r="C4" t="inlineStr">
         <is>
           <t>P</t>
         </is>
@@ -427,41 +464,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>rudraksh</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>70</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
           <t>P</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>rahul</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>44</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="A6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>xyz</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>122</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="A7" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>